<commit_message>
Code enhanced and generated output of first half
</commit_message>
<xml_diff>
--- a/start_timestamp_estimation.xlsx
+++ b/start_timestamp_estimation.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
   <si>
     <t>out</t>
   </si>
@@ -47,11 +48,17 @@
   <si>
     <t>est. start time stamp</t>
   </si>
+  <si>
+    <t>diff</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -94,7 +101,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -132,12 +139,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -156,6 +187,17 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -174,6 +216,17 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -521,7 +574,7 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -543,8 +596,11 @@
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +615,7 @@
         <v>191758000000000</v>
       </c>
       <c r="E2" s="1">
-        <f>B2-D2</f>
+        <f t="shared" ref="E2:E7" si="0">B2-D2</f>
         <v>1.07494104263897E+16</v>
       </c>
       <c r="F2" s="1">
@@ -570,8 +626,12 @@
         <f>(B2-F2)*0.000000000001</f>
         <v>191.89045233305001</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="2">
+        <f>C2-G2</f>
+        <v>-0.13245233304999715</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -582,11 +642,11 @@
         <v>215.215</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D7" si="0">C3*1000000000000</f>
+        <f t="shared" ref="D3:D7" si="1">C3*1000000000000</f>
         <v>215215000000000</v>
       </c>
       <c r="E3" s="1">
-        <f>B3-D3</f>
+        <f t="shared" si="0"/>
         <v>1.07492853799003E+16</v>
       </c>
       <c r="F3" s="1">
@@ -594,11 +654,15 @@
         <v>1.074927797405665E+16</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G7" si="1">(B3-F3)*0.000000000001</f>
+        <f t="shared" ref="G3:G7" si="2">(B3-F3)*0.000000000001</f>
         <v>215.22240584364999</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H8" si="3">C3-G3</f>
+        <v>-7.405843649991084E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,11 +673,11 @@
         <v>221.88800000000001</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>221888000000000</v>
       </c>
       <c r="E4" s="1">
-        <f>B4-D4</f>
+        <f t="shared" si="0"/>
         <v>1.0749202935578E+16</v>
       </c>
       <c r="F4" s="1">
@@ -621,11 +685,15 @@
         <v>1.074927797405665E+16</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>221.81296152134999</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="2">
+        <f t="shared" si="3"/>
+        <v>7.5038478650014895E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,11 +704,11 @@
         <v>400</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>400000000000000</v>
       </c>
       <c r="E5" s="1">
-        <f>B5-D5</f>
+        <f t="shared" si="0"/>
         <v>1.07492604166291E+16</v>
       </c>
       <c r="F5" s="1">
@@ -648,11 +716,15 @@
         <v>1.074927797405665E+16</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>399.98244257245</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7557427550002558E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,11 +735,11 @@
         <v>427.99400000000003</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>427994000000000</v>
       </c>
       <c r="E6" s="1">
-        <f>B6-D6</f>
+        <f t="shared" si="0"/>
         <v>1.07492630936426E+16</v>
       </c>
       <c r="F6" s="1">
@@ -675,11 +747,15 @@
         <v>1.074927797405665E+16</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>427.97911958595</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="2">
+        <f t="shared" si="3"/>
+        <v>1.4880414050026047E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="B7" s="1">
         <v>1.11780735922002E+16</v>
       </c>
@@ -687,11 +763,11 @@
         <v>428.82799999999997</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>428828000000000</v>
       </c>
       <c r="E7" s="1">
-        <f>B7-D7</f>
+        <f t="shared" si="0"/>
         <v>1.07492455922002E+16</v>
       </c>
       <c r="F7" s="1">
@@ -699,8 +775,350 @@
         <v>1.074927797405665E+16</v>
       </c>
       <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>428.79561814354997</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="3"/>
+        <v>3.2381856450001578E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="H8" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1">
+        <f>AVERAGE(H2:H100)</f>
+        <v>-1.9946513576643257E-12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.31114335664063E+16</v>
+      </c>
+      <c r="C2" s="2">
+        <v>26.158999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2*1000000000000</f>
+        <v>26159000000000</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ref="E2:E10" si="0">B2-D2</f>
+        <v>1.30852745664063E+16</v>
+      </c>
+      <c r="F2" s="1">
+        <f>AVERAGE(E$2:E91)</f>
+        <v>1.3085193764021898E+16</v>
+      </c>
+      <c r="G2" s="2">
+        <f>(B2-F2)*0.000000000001</f>
+        <v>26.239802384402001</v>
+      </c>
+      <c r="H2" s="2">
+        <f>C2-G2</f>
+        <v>-8.0802384402002048E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.31439212347383E+16</v>
+      </c>
+      <c r="C3" s="2">
+        <v>58.725000000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D10" si="1">C3*1000000000000</f>
+        <v>58725000000000</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="0"/>
+        <v>1.30851962347383E+16</v>
+      </c>
+      <c r="F3" s="1">
+        <f>AVERAGE(E$2:E96)</f>
+        <v>1.3085193764021898E+16</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G10" si="2">(B3-F3)*0.000000000001</f>
+        <v>58.727470716401996</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H10" si="3">C3-G3</f>
+        <v>-2.4707164019943662E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.31518868650824E+16</v>
+      </c>
+      <c r="C4" s="2">
+        <v>66.632999999999996</v>
+      </c>
+      <c r="D4" s="1">
         <f t="shared" si="1"/>
-        <v>428.79561814354997</v>
+        <v>66632999999999.992</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.30852538650824E+16</v>
+      </c>
+      <c r="F4" s="1">
+        <f>AVERAGE(E$2:E99)</f>
+        <v>1.3085193764021898E+16</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="2"/>
+        <v>66.693101060502002</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="3"/>
+        <v>-6.0101060502006476E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.31993186657982E+16</v>
+      </c>
+      <c r="C5" s="2">
+        <v>114.18</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>114180000000000</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.30851386657982E+16</v>
+      </c>
+      <c r="F5" s="1">
+        <f>AVERAGE(E$2:E100)</f>
+        <v>1.3085193764021898E+16</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="2"/>
+        <v>114.124901776302</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="3"/>
+        <v>5.5098223698010429E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.32034970632945E+16</v>
+      </c>
+      <c r="C6" s="2">
+        <v>118.28400000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="1"/>
+        <v>118284000000000</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.30852130632945E+16</v>
+      </c>
+      <c r="F6" s="1">
+        <f>AVERAGE(E$2:E101)</f>
+        <v>1.3085193764021898E+16</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>118.303299272602</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.9299272601998041E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.32141557912542E+16</v>
+      </c>
+      <c r="C7" s="2">
+        <v>128.96199999999999</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="1"/>
+        <v>128961999999999.98</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.30851937912542E+16</v>
+      </c>
+      <c r="F7" s="1">
+        <f>AVERAGE(E$2:E102)</f>
+        <v>1.3085193764021898E+16</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>128.96202723230201</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="3"/>
+        <v>-2.7232302016955146E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.3230487432342E+16</v>
+      </c>
+      <c r="C8" s="2">
+        <v>145.27799999999999</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>145278000000000</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3085209432342E+16</v>
+      </c>
+      <c r="F8" s="1">
+        <f>AVERAGE(E$2:E103)</f>
+        <v>1.3085193764021898E+16</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="2"/>
+        <v>145.293668320102</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.5668320102008693E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.33451975232004E+16</v>
+      </c>
+      <c r="C9" s="2">
+        <v>260.09300000000002</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="1"/>
+        <v>260093000000000.03</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.30851045232004E+16</v>
+      </c>
+      <c r="F9" s="1">
+        <f>AVERAGE(E$2:E104)</f>
+        <v>1.3085193764021898E+16</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>260.00375917850198</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="3"/>
+        <v>8.9240821498037803E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.34344747340808E+16</v>
+      </c>
+      <c r="C10" s="2">
+        <v>349.315</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>349315000000000</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.30851597340808E+16</v>
+      </c>
+      <c r="F10" s="1">
+        <f>AVERAGE(E$2:E105)</f>
+        <v>1.3085193764021898E+16</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>349.28097005890197</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="3"/>
+        <v>3.4029941098026484E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>